<commit_message>
Login interface language config
</commit_message>
<xml_diff>
--- a/WebRoot/locale/locale-en.xlsx
+++ b/WebRoot/locale/locale-en.xlsx
@@ -1,28 +1,375 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211" fullCalcOnLoad="1"/>
+  <calcPr calcId="122211"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="83">
+  <si>
+    <t>myself</t>
+  </si>
+  <si>
+    <t>dateFormat</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>yyyy-MM-dd HH:mm:ss</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>deviceName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>刷新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>refresh</t>
+  </si>
+  <si>
+    <t>loading</t>
+  </si>
+  <si>
+    <t>数据加载中，请稍后…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>export</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>导出</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>showHistory</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查看历史</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>online</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>在线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>offline</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>离线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>run</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>stop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>停止</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>noData</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>无数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>工况诊断</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>通信状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>运行状态</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>井筒分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地面分析</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>趋势曲线</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>动态数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备控制</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>设备信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>没有记录可显示</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>上一页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>下一页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>最后页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>第一页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>共{0}页</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>总记录数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>信息提示</t>
+  </si>
+  <si>
+    <t>信息</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>后台获取数据失败</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位类别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>全部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位编码</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位级别</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>单位说明</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询单位信息…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>创建</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>保存</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>修改</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>取消</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>是</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>否</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>确认</t>
+  </si>
+  <si>
+    <t>名称</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>查询</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收缩</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>收缩全部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>展开</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>展开全部</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>IDX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ITEM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>VALUE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>userLogin</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enterUserName</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>rememberPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>contact</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enterPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>user login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter user name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>enter password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>remember password</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forgerPassword</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>forger password?</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Contact the administrator to reset the password.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>login</t>
+  </si>
+  <si>
+    <t>login</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logining</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>logining…</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -34,7 +381,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -42,23 +389,45 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -343,37 +712,872 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C106"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="22.109375" customWidth="1"/>
+    <col min="3" max="3" width="57" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1"/>
+      <c r="C12" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1"/>
+      <c r="C45" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="1">
+        <v>11</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="1">
+        <v>12</v>
+      </c>
+      <c r="B47" s="1"/>
+      <c r="C47" s="1"/>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="1">
+        <v>13</v>
+      </c>
+      <c r="B48" s="1"/>
+      <c r="C48" s="1"/>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="1">
+        <v>14</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="1">
+        <v>15</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="1">
+        <v>16</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="1">
+        <v>17</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="1">
+        <v>18</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="1">
+        <v>19</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="1">
+        <v>20</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="1">
+        <v>21</v>
+      </c>
+      <c r="B56" s="1"/>
+      <c r="C56" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="1">
+        <v>22</v>
+      </c>
+      <c r="B57" s="1"/>
+      <c r="C57" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="1">
+        <v>23</v>
+      </c>
+      <c r="B58" s="1"/>
+      <c r="C58" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="1">
+        <v>24</v>
+      </c>
+      <c r="B59" s="1"/>
+      <c r="C59" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="1">
+        <v>25</v>
+      </c>
+      <c r="B60" s="1"/>
+      <c r="C60" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="1">
+        <v>26</v>
+      </c>
+      <c r="B61" s="1"/>
+      <c r="C61" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="1">
+        <v>27</v>
+      </c>
+      <c r="B62" s="1"/>
+      <c r="C62" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="1">
+        <v>28</v>
+      </c>
+      <c r="B63" s="1"/>
+      <c r="C63" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="1">
+        <v>29</v>
+      </c>
+      <c r="B64" s="1"/>
+      <c r="C64" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" s="1"/>
+      <c r="B65" s="1"/>
+      <c r="C65" s="1"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" s="1"/>
+      <c r="B66" s="1"/>
+      <c r="C66" s="1"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="1"/>
+      <c r="B67" s="1"/>
+      <c r="C67" s="1"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="1"/>
+      <c r="B68" s="1"/>
+      <c r="C68" s="1"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="1"/>
+      <c r="B69" s="1"/>
+      <c r="C69" s="1"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="1"/>
+      <c r="B70" s="1"/>
+      <c r="C70" s="1"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" s="1"/>
+      <c r="B71" s="1"/>
+      <c r="C71" s="1"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" s="1"/>
+      <c r="B72" s="1"/>
+      <c r="C72" s="1"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" s="1"/>
+      <c r="B73" s="1"/>
+      <c r="C73" s="1"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="1"/>
+      <c r="B74" s="1"/>
+      <c r="C74" s="1"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="1"/>
+      <c r="B75" s="1"/>
+      <c r="C75" s="1"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="1"/>
+      <c r="B76" s="1"/>
+      <c r="C76" s="1"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="1"/>
+      <c r="B77" s="1"/>
+      <c r="C77" s="1"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="1"/>
+      <c r="B78" s="1"/>
+      <c r="C78" s="1"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="1"/>
+      <c r="B79" s="1"/>
+      <c r="C79" s="1"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="1"/>
+      <c r="B80" s="1"/>
+      <c r="C80" s="1"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="1"/>
+      <c r="B81" s="1"/>
+      <c r="C81" s="1"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="1"/>
+      <c r="B82" s="1"/>
+      <c r="C82" s="1"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="1"/>
+      <c r="B83" s="1"/>
+      <c r="C83" s="1"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="1"/>
+      <c r="B84" s="1"/>
+      <c r="C84" s="1"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="1"/>
+      <c r="B85" s="1"/>
+      <c r="C85" s="1"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="1"/>
+      <c r="B86" s="1"/>
+      <c r="C86" s="1"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="1"/>
+      <c r="B87" s="1"/>
+      <c r="C87" s="1"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="1"/>
+      <c r="B88" s="1"/>
+      <c r="C88" s="1"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="1"/>
+      <c r="B89" s="1"/>
+      <c r="C89" s="1"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" s="1"/>
+      <c r="B90" s="1"/>
+      <c r="C90" s="1"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" s="1"/>
+      <c r="B91" s="1"/>
+      <c r="C91" s="1"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" s="1"/>
+      <c r="B92" s="1"/>
+      <c r="C92" s="1"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" s="1"/>
+      <c r="B93" s="1"/>
+      <c r="C93" s="1"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" s="1"/>
+      <c r="B94" s="1"/>
+      <c r="C94" s="1"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" s="1"/>
+      <c r="B95" s="1"/>
+      <c r="C95" s="1"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" s="1"/>
+      <c r="B96" s="1"/>
+      <c r="C96" s="1"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A97" s="1"/>
+      <c r="B97" s="1"/>
+      <c r="C97" s="1"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="1"/>
+      <c r="B98" s="1"/>
+      <c r="C98" s="1"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="1"/>
+      <c r="B99" s="1"/>
+      <c r="C99" s="1"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="1"/>
+      <c r="B100" s="1"/>
+      <c r="C100" s="1"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="1"/>
+      <c r="B102" s="1"/>
+      <c r="C102" s="1"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="1"/>
+      <c r="B103" s="1"/>
+      <c r="C103" s="1"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="1"/>
+      <c r="B104" s="1"/>
+      <c r="C104" s="1"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="1"/>
+      <c r="B105" s="1"/>
+      <c r="C105" s="1"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="1"/>
+      <c r="B106" s="1"/>
+      <c r="C106" s="1"/>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
   <sheetData/>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>